<commit_message>
Fixed comments and spelling mistake in comparison.
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarkoIvan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kiki\Faks\2semestar_dipl\Bioinformatika_1\Projekt\git_kod\bioinformatics-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E6AEC1-3DE5-4E9A-A7FA-EACA934C46DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C6B8D5-99C2-40B2-A868-EBF4F3274255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA05282B-FBA7-4B3B-A849-52D45BC5F707}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
   <si>
     <t>300_O (ms)</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>DECOMPRESSION (E-coli)</t>
+  </si>
+  <si>
+    <t>300000_O (kB)</t>
   </si>
 </sst>
 </file>
@@ -567,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB87F824-6484-41C7-A212-CAD65F7360FA}">
   <dimension ref="A1:AD46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1089,7 @@
         <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="N10" t="s">
         <v>24</v>
@@ -1579,7 +1582,7 @@
         <v>7.1903999999999995</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:AD21" si="2">AVERAGE(C16:C20)</f>
+        <f t="shared" ref="C21:AC21" si="2">AVERAGE(C16:C20)</f>
         <v>5.1584000000000003</v>
       </c>
       <c r="E21">

</xml_diff>